<commit_message>
Completed squaring off futures analysis
</commit_message>
<xml_diff>
--- a/financial_derivates_futures_options/reliance_future_dataset.xlsx
+++ b/financial_derivates_futures_options/reliance_future_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_derivates/financial_derivates_futures_options/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ABCCD9-6240-A14F-B2E0-3FC8A6C9014F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE12226-85F9-4048-9F09-3FB4B5FC3BAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{0392D1FD-9317-0E42-BE43-26A2C5832841}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{0392D1FD-9317-0E42-BE43-26A2C5832841}"/>
   </bookViews>
   <sheets>
     <sheet name="Hedging &amp; Payoff" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="58">
   <si>
     <t xml:space="preserve">DATE </t>
   </si>
@@ -182,12 +182,36 @@
   <si>
     <t>Final price at which I buy 1 share</t>
   </si>
+  <si>
+    <t>Trading Data and Payoff</t>
+  </si>
+  <si>
+    <t>Squaring off Futures</t>
+  </si>
+  <si>
+    <t>Existing Futures contract without settlement (before expiry)</t>
+  </si>
+  <si>
+    <t>You expected the prices to increase, but they are decreasing</t>
+  </si>
+  <si>
+    <t>or You no longer hold the asset</t>
+  </si>
+  <si>
+    <t>thus you go Short Futures at price</t>
+  </si>
+  <si>
+    <t>On 29th May, you want to exit</t>
+  </si>
+  <si>
+    <t>29 May Pay off from Futures Profit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -199,6 +223,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -245,13 +277,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2278,10 +2311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BC4E22-B584-1541-8E78-A80684393DC6}">
-  <dimension ref="B33:F50"/>
+  <dimension ref="A7:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2291,119 +2324,181 @@
     <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1427.8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="3">
+        <v>250</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="3">
+        <f>C16*C18</f>
+        <v>356950</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="3">
+        <f>'Futures Data'!D21</f>
+        <v>1426.95</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="5">
+        <f>'Futures Data'!D60</f>
+        <v>1717.9</v>
+      </c>
+      <c r="C25" s="5">
+        <f>C16</f>
+        <v>1427.8</v>
+      </c>
+      <c r="D25" s="5">
+        <f>B25-C25</f>
+        <v>290.10000000000014</v>
+      </c>
+      <c r="E25" s="5">
+        <f>-B25</f>
+        <v>-1717.9</v>
+      </c>
+      <c r="F25" s="5">
+        <f>E25+D25</f>
+        <v>-1427.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>34</v>
+      <c r="B34" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="3">
+        <f>'Futures Data'!C41</f>
+        <v>1459.15</v>
+      </c>
+      <c r="D34" t="str">
+        <f>D16</f>
+        <v>Rs per share</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="3">
-        <v>1427.8</v>
-      </c>
-      <c r="D41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="3">
-        <v>250</v>
-      </c>
-      <c r="D43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="3">
-        <f>C41*C43</f>
-        <v>356950</v>
-      </c>
-      <c r="D45" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="3">
-        <f>'Futures Data'!D21</f>
-        <v>1426.95</v>
-      </c>
-      <c r="D47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B49" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B50" s="5">
-        <f>'Futures Data'!D60</f>
-        <v>1717.9</v>
-      </c>
-      <c r="C50" s="5">
-        <f>C41</f>
-        <v>1427.8</v>
-      </c>
-      <c r="D50" s="5">
-        <f>B50-C50</f>
-        <v>290.10000000000014</v>
-      </c>
-      <c r="E50" s="5">
-        <f>-B50</f>
-        <v>-1717.9</v>
-      </c>
-      <c r="F50" s="5">
-        <f>E50+D50</f>
-        <v>-1427.8</v>
+      <c r="B36" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="2">
+        <f>C34-C16</f>
+        <v>31.350000000000136</v>
+      </c>
+      <c r="D36" t="str">
+        <f>D34</f>
+        <v>Rs per share</v>
       </c>
     </row>
   </sheetData>
@@ -2415,8 +2510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD808CD-D11A-2A44-A93C-B1CA4C3A65E2}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Completed Rolling Over Hedge analysis
</commit_message>
<xml_diff>
--- a/financial_derivates_futures_options/reliance_future_dataset.xlsx
+++ b/financial_derivates_futures_options/reliance_future_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_derivates/financial_derivates_futures_options/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE12226-85F9-4048-9F09-3FB4B5FC3BAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC6943A-13C6-334A-A479-F307D26C2CCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{0392D1FD-9317-0E42-BE43-26A2C5832841}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Futures Data" sheetId="2" r:id="rId2"/>
     <sheet name="Futures All Data" sheetId="1" r:id="rId3"/>
     <sheet name="Equity Data" sheetId="3" r:id="rId4"/>
+    <sheet name="June - Sep Data" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Futures Data'!$A$1:$C$1</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="76">
   <si>
     <t xml:space="preserve">DATE </t>
   </si>
@@ -205,6 +206,60 @@
   </si>
   <si>
     <t>29 May Pay off from Futures Profit</t>
+  </si>
+  <si>
+    <t>Stock Price</t>
+  </si>
+  <si>
+    <t>Roll over Hedge</t>
+  </si>
+  <si>
+    <t>We are 9th Apr 2020, and RIL shares are continuously increasing</t>
+  </si>
+  <si>
+    <t>I wish to buy shares of RIL, but will have money in Sep 2020</t>
+  </si>
+  <si>
+    <t>However, what if prices becomes very high</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>9th Apr</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Future Prices </t>
+  </si>
+  <si>
+    <t>Payoff</t>
+  </si>
+  <si>
+    <t>Long June Futures</t>
+  </si>
+  <si>
+    <t>25th June</t>
+  </si>
+  <si>
+    <t>Sell June Futures</t>
+  </si>
+  <si>
+    <t>26th June</t>
+  </si>
+  <si>
+    <t>24th Sep</t>
+  </si>
+  <si>
+    <t>Total Pay off</t>
+  </si>
+  <si>
+    <t>Futures Payoff</t>
+  </si>
+  <si>
+    <t>Spot price on 24th Sep</t>
   </si>
 </sst>
 </file>
@@ -597,6 +652,9 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>44007</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2311,15 +2369,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BC4E22-B584-1541-8E78-A80684393DC6}">
-  <dimension ref="A7:F36"/>
+  <dimension ref="A7:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="81.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2470,12 +2529,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
         <v>55</v>
       </c>
@@ -2488,7 +2547,7 @@
         <v>Rs per share</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>57</v>
       </c>
@@ -2499,6 +2558,136 @@
       <c r="D36" t="str">
         <f>D34</f>
         <v>Rs per share</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="2">
+        <f>'Futures Data'!C9</f>
+        <v>1230</v>
+      </c>
+      <c r="E45" s="2">
+        <f>'Futures Data'!D9</f>
+        <v>1219.95</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="2">
+        <f>'Futures Data'!C60</f>
+        <v>1717.9</v>
+      </c>
+      <c r="F46" s="2">
+        <f>D46-D45</f>
+        <v>487.90000000000009</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="2">
+        <f>'Futures Data'!C61</f>
+        <v>1748.3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="2">
+        <f>'Futures Data'!C125</f>
+        <v>2181.1999999999998</v>
+      </c>
+      <c r="F48" s="2">
+        <f>D48-D47</f>
+        <v>432.89999999999986</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>73</v>
+      </c>
+      <c r="F50" s="2">
+        <f>F48+F46</f>
+        <v>920.8</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D52" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F52" s="2">
+        <f>F50</f>
+        <v>920.8</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>75</v>
+      </c>
+      <c r="F53" s="2">
+        <f>'Futures Data'!D125</f>
+        <v>2181.1999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F54" s="2">
+        <f>F53-F52</f>
+        <v>1260.3999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2508,10 +2697,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD808CD-D11A-2A44-A93C-B1CA4C3A65E2}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D61" sqref="D61:D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3359,6 +3548,916 @@
       </c>
       <c r="D60" s="2">
         <v>1717.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>44008</v>
+      </c>
+      <c r="B61" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1748.3</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1741.65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>44011</v>
+      </c>
+      <c r="B62" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1722.95</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1723.15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>44012</v>
+      </c>
+      <c r="B63" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C63" s="2">
+        <v>1705</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1704.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B64" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C64" s="2">
+        <v>1741.6</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1737.6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>44014</v>
+      </c>
+      <c r="B65" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C65" s="2">
+        <v>1767.85</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1760.35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>44015</v>
+      </c>
+      <c r="B66" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C66" s="2">
+        <v>1794</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1787.9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>44018</v>
+      </c>
+      <c r="B67" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C67" s="2">
+        <v>1858.55</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1851.8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>44019</v>
+      </c>
+      <c r="B68" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C68" s="2">
+        <v>1838.95</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1823.45</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>44020</v>
+      </c>
+      <c r="B69" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C69" s="2">
+        <v>1813.6</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>44021</v>
+      </c>
+      <c r="B70" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C70" s="2">
+        <v>1836.5</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1824.25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>44022</v>
+      </c>
+      <c r="B71" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C71" s="2">
+        <v>1895.7</v>
+      </c>
+      <c r="D71" s="2">
+        <v>1878.05</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>44025</v>
+      </c>
+      <c r="B72" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C72" s="2">
+        <v>1950.35</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>44026</v>
+      </c>
+      <c r="B73" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C73" s="2">
+        <v>1932.35</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>44027</v>
+      </c>
+      <c r="B74" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C74" s="2">
+        <v>1861.9</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>44028</v>
+      </c>
+      <c r="B75" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C75" s="2">
+        <v>1853.6</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1843.4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>44029</v>
+      </c>
+      <c r="B76" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C76" s="2">
+        <v>1928.15</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1911.7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>44032</v>
+      </c>
+      <c r="B77" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C77" s="2">
+        <v>1933.3</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1919.9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>44033</v>
+      </c>
+      <c r="B78" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C78" s="2">
+        <v>1984.05</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1971.55</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>44034</v>
+      </c>
+      <c r="B79" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C79" s="2">
+        <v>2013.35</v>
+      </c>
+      <c r="D79" s="2">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>44035</v>
+      </c>
+      <c r="B80" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C80" s="2">
+        <v>2070.15</v>
+      </c>
+      <c r="D80" s="2">
+        <v>2057.8000000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>44036</v>
+      </c>
+      <c r="B81" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C81" s="2">
+        <v>2159</v>
+      </c>
+      <c r="D81" s="2">
+        <v>2146.15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>44039</v>
+      </c>
+      <c r="B82" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C82" s="2">
+        <v>2166.4499999999998</v>
+      </c>
+      <c r="D82" s="2">
+        <v>2156.1999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>44040</v>
+      </c>
+      <c r="B83" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C83" s="2">
+        <v>2187</v>
+      </c>
+      <c r="D83" s="2">
+        <v>2177.6999999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>44041</v>
+      </c>
+      <c r="B84" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C84" s="2">
+        <v>2114.15</v>
+      </c>
+      <c r="D84" s="2">
+        <v>2096.65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>44042</v>
+      </c>
+      <c r="B85" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C85" s="2">
+        <v>2120.5</v>
+      </c>
+      <c r="D85" s="2">
+        <v>2108.85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>44043</v>
+      </c>
+      <c r="B86" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C86" s="2">
+        <v>2084.5500000000002</v>
+      </c>
+      <c r="D86" s="2">
+        <v>2067.1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>44046</v>
+      </c>
+      <c r="B87" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C87" s="2">
+        <v>2025.8</v>
+      </c>
+      <c r="D87" s="2">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>44047</v>
+      </c>
+      <c r="B88" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C88" s="2">
+        <v>2167.8000000000002</v>
+      </c>
+      <c r="D88" s="2">
+        <v>2150.6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>44048</v>
+      </c>
+      <c r="B89" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C89" s="2">
+        <v>2141.15</v>
+      </c>
+      <c r="D89" s="2">
+        <v>2126.4499999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>44049</v>
+      </c>
+      <c r="B90" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C90" s="2">
+        <v>2149.9</v>
+      </c>
+      <c r="D90" s="2">
+        <v>2134.1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>44050</v>
+      </c>
+      <c r="B91" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C91" s="2">
+        <v>2163.6</v>
+      </c>
+      <c r="D91" s="2">
+        <v>2146.4499999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>44053</v>
+      </c>
+      <c r="B92" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C92" s="2">
+        <v>2138.35</v>
+      </c>
+      <c r="D92" s="2">
+        <v>2119.85</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>44054</v>
+      </c>
+      <c r="B93" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C93" s="2">
+        <v>2150.65</v>
+      </c>
+      <c r="D93" s="2">
+        <v>2133.8000000000002</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>44055</v>
+      </c>
+      <c r="B94" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C94" s="2">
+        <v>2144.1999999999998</v>
+      </c>
+      <c r="D94" s="2">
+        <v>2127.6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>44056</v>
+      </c>
+      <c r="B95" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C95" s="2">
+        <v>2137.75</v>
+      </c>
+      <c r="D95" s="2">
+        <v>2122.0500000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>44057</v>
+      </c>
+      <c r="B96" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C96" s="2">
+        <v>2128</v>
+      </c>
+      <c r="D96" s="2">
+        <v>2113.8000000000002</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>44060</v>
+      </c>
+      <c r="B97" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C97" s="2">
+        <v>2104.25</v>
+      </c>
+      <c r="D97" s="2">
+        <v>2091.35</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>44061</v>
+      </c>
+      <c r="B98" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C98" s="2">
+        <v>2131.5500000000002</v>
+      </c>
+      <c r="D98" s="2">
+        <v>2118.5500000000002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>44062</v>
+      </c>
+      <c r="B99" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C99" s="2">
+        <v>2145.25</v>
+      </c>
+      <c r="D99" s="2">
+        <v>2131.5500000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>44063</v>
+      </c>
+      <c r="B100" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C100" s="2">
+        <v>2108.15</v>
+      </c>
+      <c r="D100" s="2">
+        <v>2097.0500000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>44064</v>
+      </c>
+      <c r="B101" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C101" s="2">
+        <v>2093.8000000000002</v>
+      </c>
+      <c r="D101" s="2">
+        <v>2081.85</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>44067</v>
+      </c>
+      <c r="B102" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C102" s="2">
+        <v>2108.3000000000002</v>
+      </c>
+      <c r="D102" s="2">
+        <v>2095.75</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>44068</v>
+      </c>
+      <c r="B103" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C103" s="2">
+        <v>2094</v>
+      </c>
+      <c r="D103" s="2">
+        <v>2082.1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>44069</v>
+      </c>
+      <c r="B104" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C104" s="2">
+        <v>2145.0500000000002</v>
+      </c>
+      <c r="D104" s="2">
+        <v>2137.3000000000002</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>44070</v>
+      </c>
+      <c r="B105" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C105" s="2">
+        <v>2117.1</v>
+      </c>
+      <c r="D105" s="2">
+        <v>2110.6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>44071</v>
+      </c>
+      <c r="B106" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C106" s="2">
+        <v>2127.1</v>
+      </c>
+      <c r="D106" s="2">
+        <v>2116.15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>44074</v>
+      </c>
+      <c r="B107" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C107" s="2">
+        <v>2088.75</v>
+      </c>
+      <c r="D107" s="2">
+        <v>2080.6999999999998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B108" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C108" s="2">
+        <v>2100.15</v>
+      </c>
+      <c r="D108" s="2">
+        <v>2087.25</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>44076</v>
+      </c>
+      <c r="B109" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C109" s="2">
+        <v>2139.5500000000002</v>
+      </c>
+      <c r="D109" s="2">
+        <v>2128.1999999999998</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>44077</v>
+      </c>
+      <c r="B110" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C110" s="2">
+        <v>2120</v>
+      </c>
+      <c r="D110" s="2">
+        <v>2112.1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>44078</v>
+      </c>
+      <c r="B111" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C111" s="2">
+        <v>2083.8000000000002</v>
+      </c>
+      <c r="D111" s="2">
+        <v>2077.25</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>44081</v>
+      </c>
+      <c r="B112" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C112" s="2">
+        <v>2097.1</v>
+      </c>
+      <c r="D112" s="2">
+        <v>2082.65</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>44082</v>
+      </c>
+      <c r="B113" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C113" s="2">
+        <v>2115</v>
+      </c>
+      <c r="D113" s="2">
+        <v>2107.1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>44083</v>
+      </c>
+      <c r="B114" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C114" s="2">
+        <v>2169.0500000000002</v>
+      </c>
+      <c r="D114" s="2">
+        <v>2161.35</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>44084</v>
+      </c>
+      <c r="B115" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C115" s="2">
+        <v>2316.3000000000002</v>
+      </c>
+      <c r="D115" s="2">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <v>44085</v>
+      </c>
+      <c r="B116" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C116" s="2">
+        <v>2320.1</v>
+      </c>
+      <c r="D116" s="2">
+        <v>2319.75</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <v>44088</v>
+      </c>
+      <c r="B117" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C117" s="2">
+        <v>2303.75</v>
+      </c>
+      <c r="D117" s="2">
+        <v>2302.5500000000002</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>44089</v>
+      </c>
+      <c r="B118" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C118" s="2">
+        <v>2320.5</v>
+      </c>
+      <c r="D118" s="2">
+        <v>2318.85</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>44090</v>
+      </c>
+      <c r="B119" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C119" s="2">
+        <v>2330.85</v>
+      </c>
+      <c r="D119" s="2">
+        <v>2324.5500000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>44091</v>
+      </c>
+      <c r="B120" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C120" s="2">
+        <v>2305.6999999999998</v>
+      </c>
+      <c r="D120" s="2">
+        <v>2298.75</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>44092</v>
+      </c>
+      <c r="B121" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C121" s="2">
+        <v>2307.8000000000002</v>
+      </c>
+      <c r="D121" s="2">
+        <v>2305.6999999999998</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>44095</v>
+      </c>
+      <c r="B122" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C122" s="2">
+        <v>2259.85</v>
+      </c>
+      <c r="D122" s="2">
+        <v>2255.85</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>44096</v>
+      </c>
+      <c r="B123" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C123" s="2">
+        <v>2218.3000000000002</v>
+      </c>
+      <c r="D123" s="2">
+        <v>2211.15</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>44097</v>
+      </c>
+      <c r="B124" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C124" s="2">
+        <v>2237.5500000000002</v>
+      </c>
+      <c r="D124" s="2">
+        <v>2230.8000000000002</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>44098</v>
+      </c>
+      <c r="B125" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C125" s="2">
+        <v>2181.1999999999998</v>
+      </c>
+      <c r="D125" s="2">
+        <v>2181.1999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -8874,4 +9973,1702 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8E89BA-A5D1-FB4A-9C08-771B649AEA27}">
+  <dimension ref="A1:D319"/>
+  <sheetViews>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>44008</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1748.3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1741.65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>44011</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1722.95</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1723.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>44012</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1705</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1704.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1741.6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1737.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>44014</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1767.85</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1760.35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>44015</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1794</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1787.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>44018</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1858.55</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1851.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>44019</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1838.95</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1823.45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>44020</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1813.6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>44021</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1836.5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1824.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>44022</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1895.7</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1878.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>44025</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1950.35</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>44026</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1932.35</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>44027</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1861.9</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>44028</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1853.6</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1843.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>44029</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1928.15</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1911.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>44032</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1933.3</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1919.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>44033</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1984.05</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1971.55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>44034</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2013.35</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>44035</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2070.15</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2057.8000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>44036</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2159</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2146.15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>44039</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2166.4499999999998</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2156.1999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>44040</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2187</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2177.6999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>44041</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2114.15</v>
+      </c>
+      <c r="D25" s="2">
+        <v>2096.65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>44042</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2120.5</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2108.85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>44043</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2084.5500000000002</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2067.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>44046</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2025.8</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>44047</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2167.8000000000002</v>
+      </c>
+      <c r="D29" s="2">
+        <v>2150.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>44048</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2141.15</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2126.4499999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>44049</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2149.9</v>
+      </c>
+      <c r="D31" s="2">
+        <v>2134.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>44050</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2163.6</v>
+      </c>
+      <c r="D32" s="2">
+        <v>2146.4499999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>44053</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2138.35</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2119.85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>44054</v>
+      </c>
+      <c r="B34" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2150.65</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2133.8000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>44055</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2144.1999999999998</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2127.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>44056</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C36" s="2">
+        <v>2137.75</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2122.0500000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>44057</v>
+      </c>
+      <c r="B37" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2128</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2113.8000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>44060</v>
+      </c>
+      <c r="B38" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2104.25</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2091.35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>44061</v>
+      </c>
+      <c r="B39" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2131.5500000000002</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2118.5500000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>44062</v>
+      </c>
+      <c r="B40" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2145.25</v>
+      </c>
+      <c r="D40" s="2">
+        <v>2131.5500000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>44063</v>
+      </c>
+      <c r="B41" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2108.15</v>
+      </c>
+      <c r="D41" s="2">
+        <v>2097.0500000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>44064</v>
+      </c>
+      <c r="B42" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2093.8000000000002</v>
+      </c>
+      <c r="D42" s="2">
+        <v>2081.85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>44067</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C43" s="2">
+        <v>2108.3000000000002</v>
+      </c>
+      <c r="D43" s="2">
+        <v>2095.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>44068</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2094</v>
+      </c>
+      <c r="D44" s="2">
+        <v>2082.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>44069</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2145.0500000000002</v>
+      </c>
+      <c r="D45" s="2">
+        <v>2137.3000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>44070</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2117.1</v>
+      </c>
+      <c r="D46" s="2">
+        <v>2110.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>44071</v>
+      </c>
+      <c r="B47" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C47" s="2">
+        <v>2127.1</v>
+      </c>
+      <c r="D47" s="2">
+        <v>2116.15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>44074</v>
+      </c>
+      <c r="B48" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C48" s="2">
+        <v>2088.75</v>
+      </c>
+      <c r="D48" s="2">
+        <v>2080.6999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B49" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C49" s="2">
+        <v>2100.15</v>
+      </c>
+      <c r="D49" s="2">
+        <v>2087.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>44076</v>
+      </c>
+      <c r="B50" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C50" s="2">
+        <v>2139.5500000000002</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2128.1999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>44077</v>
+      </c>
+      <c r="B51" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C51" s="2">
+        <v>2120</v>
+      </c>
+      <c r="D51" s="2">
+        <v>2112.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>44078</v>
+      </c>
+      <c r="B52" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C52" s="2">
+        <v>2083.8000000000002</v>
+      </c>
+      <c r="D52" s="2">
+        <v>2077.25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>44081</v>
+      </c>
+      <c r="B53" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C53" s="2">
+        <v>2097.1</v>
+      </c>
+      <c r="D53" s="2">
+        <v>2082.65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>44082</v>
+      </c>
+      <c r="B54" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C54" s="2">
+        <v>2115</v>
+      </c>
+      <c r="D54" s="2">
+        <v>2107.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>44083</v>
+      </c>
+      <c r="B55" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C55" s="2">
+        <v>2169.0500000000002</v>
+      </c>
+      <c r="D55" s="2">
+        <v>2161.35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>44084</v>
+      </c>
+      <c r="B56" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C56" s="2">
+        <v>2316.3000000000002</v>
+      </c>
+      <c r="D56" s="2">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>44085</v>
+      </c>
+      <c r="B57" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C57" s="2">
+        <v>2320.1</v>
+      </c>
+      <c r="D57" s="2">
+        <v>2319.75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>44088</v>
+      </c>
+      <c r="B58" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C58" s="2">
+        <v>2303.75</v>
+      </c>
+      <c r="D58" s="2">
+        <v>2302.5500000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>44089</v>
+      </c>
+      <c r="B59" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C59" s="2">
+        <v>2320.5</v>
+      </c>
+      <c r="D59" s="2">
+        <v>2318.85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>44090</v>
+      </c>
+      <c r="B60" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C60" s="2">
+        <v>2330.85</v>
+      </c>
+      <c r="D60" s="2">
+        <v>2324.5500000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>44091</v>
+      </c>
+      <c r="B61" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C61" s="2">
+        <v>2305.6999999999998</v>
+      </c>
+      <c r="D61" s="2">
+        <v>2298.75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>44092</v>
+      </c>
+      <c r="B62" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C62" s="2">
+        <v>2307.8000000000002</v>
+      </c>
+      <c r="D62" s="2">
+        <v>2305.6999999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>44095</v>
+      </c>
+      <c r="B63" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C63" s="2">
+        <v>2259.85</v>
+      </c>
+      <c r="D63" s="2">
+        <v>2255.85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>44096</v>
+      </c>
+      <c r="B64" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C64" s="2">
+        <v>2218.3000000000002</v>
+      </c>
+      <c r="D64" s="2">
+        <v>2211.15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>44097</v>
+      </c>
+      <c r="B65" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C65" s="2">
+        <v>2237.5500000000002</v>
+      </c>
+      <c r="D65" s="2">
+        <v>2230.8000000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>44098</v>
+      </c>
+      <c r="B66" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C66" s="2">
+        <v>2181.1999999999998</v>
+      </c>
+      <c r="D66" s="2">
+        <v>2181.1999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D97" s="2"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D99" s="2"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D103" s="2"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D104" s="2"/>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D106" s="2"/>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D107" s="2"/>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D108" s="2"/>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D109" s="2"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D110" s="2"/>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D111" s="2"/>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D114" s="2"/>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D115" s="2"/>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D116" s="2"/>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D117" s="2"/>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D118" s="2"/>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D119" s="2"/>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D120" s="2"/>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D121" s="2"/>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D122" s="2"/>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D123" s="2"/>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D124" s="2"/>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D125" s="2"/>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D126" s="2"/>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D127" s="2"/>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D128" s="2"/>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D129" s="2"/>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D130" s="2"/>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D131" s="2"/>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D132" s="2"/>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D133" s="2"/>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D134" s="2"/>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D135" s="2"/>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D136" s="2"/>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D137" s="2"/>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D138" s="2"/>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D139" s="2"/>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D140" s="2"/>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D141" s="2"/>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D142" s="2"/>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D143" s="2"/>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D144" s="2"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D145" s="2"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D146" s="2"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D147" s="2"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D148" s="2"/>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D149" s="2"/>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D150" s="2"/>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D151" s="2"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D152" s="2"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D153" s="2"/>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D154" s="2"/>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D155" s="2"/>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D156" s="2"/>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D157" s="2"/>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D158" s="2"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D159" s="2"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D160" s="2"/>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D161" s="2"/>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D162" s="2"/>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D163" s="2"/>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D164" s="2"/>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D165" s="2"/>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D166" s="2"/>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D167" s="2"/>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D168" s="2"/>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D169" s="2"/>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D170" s="2"/>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D171" s="2"/>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D172" s="2"/>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D173" s="2"/>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D174" s="2"/>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D175" s="2"/>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D176" s="2"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D177" s="2"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D178" s="2"/>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D179" s="2"/>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D180" s="2"/>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D181" s="2"/>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D182" s="2"/>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D183" s="2"/>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D184" s="2"/>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D185" s="2"/>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D186" s="2"/>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D187" s="2"/>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D188" s="2"/>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D189" s="2"/>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D190" s="2"/>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D191" s="2"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D192" s="2"/>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D193" s="2"/>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D194" s="2"/>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D195" s="2"/>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D196" s="2"/>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D197" s="2"/>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D198" s="2"/>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D199" s="2"/>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D200" s="2"/>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D201" s="2"/>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D202" s="2"/>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D203" s="2"/>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D204" s="2"/>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D205" s="2"/>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D206" s="2"/>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D207" s="2"/>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D208" s="2"/>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D209" s="2"/>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D210" s="2"/>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D211" s="2"/>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D212" s="2"/>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D213" s="2"/>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D214" s="2"/>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D215" s="2"/>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D216" s="2"/>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D217" s="2"/>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D218" s="2"/>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D219" s="2"/>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D220" s="2"/>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D221" s="2"/>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D222" s="2"/>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D223" s="2"/>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D224" s="2"/>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D225" s="2"/>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D226" s="2"/>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D227" s="2"/>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D228" s="2"/>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D229" s="2"/>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D230" s="2"/>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D231" s="2"/>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D232" s="2"/>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D233" s="2"/>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D234" s="2"/>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D235" s="2"/>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D236" s="2"/>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D237" s="2"/>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D238" s="2"/>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D239" s="2"/>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D240" s="2"/>
+    </row>
+    <row r="241" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D241" s="2"/>
+    </row>
+    <row r="242" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D242" s="2"/>
+    </row>
+    <row r="243" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D243" s="2"/>
+    </row>
+    <row r="244" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D244" s="2"/>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D245" s="2"/>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D246" s="2"/>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D247" s="2"/>
+    </row>
+    <row r="248" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D248" s="2"/>
+    </row>
+    <row r="249" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D249" s="2"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D250" s="2"/>
+    </row>
+    <row r="251" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D251" s="2"/>
+    </row>
+    <row r="252" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D252" s="2"/>
+    </row>
+    <row r="253" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D253" s="2"/>
+    </row>
+    <row r="254" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D254" s="2"/>
+    </row>
+    <row r="255" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D255" s="2"/>
+    </row>
+    <row r="256" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D256" s="2"/>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D257" s="2"/>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D258" s="2"/>
+    </row>
+    <row r="259" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D259" s="2"/>
+    </row>
+    <row r="260" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D260" s="2"/>
+    </row>
+    <row r="261" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D261" s="2"/>
+    </row>
+    <row r="262" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D262" s="2"/>
+    </row>
+    <row r="263" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D263" s="2"/>
+    </row>
+    <row r="264" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D264" s="2"/>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D265" s="2"/>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D266" s="2"/>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D267" s="2"/>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D268" s="2"/>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D269" s="2"/>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D270" s="2"/>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D271" s="2"/>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D272" s="2"/>
+    </row>
+    <row r="273" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D273" s="2"/>
+    </row>
+    <row r="274" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D274" s="2"/>
+    </row>
+    <row r="275" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D275" s="2"/>
+    </row>
+    <row r="276" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D276" s="2"/>
+    </row>
+    <row r="277" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D277" s="2"/>
+    </row>
+    <row r="278" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D278" s="2"/>
+    </row>
+    <row r="279" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D279" s="2"/>
+    </row>
+    <row r="280" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D280" s="2"/>
+    </row>
+    <row r="281" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D281" s="2"/>
+    </row>
+    <row r="282" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D282" s="2"/>
+    </row>
+    <row r="283" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D283" s="2"/>
+    </row>
+    <row r="284" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D284" s="2"/>
+    </row>
+    <row r="285" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D285" s="2"/>
+    </row>
+    <row r="286" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D286" s="2"/>
+    </row>
+    <row r="287" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D287" s="2"/>
+    </row>
+    <row r="288" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D288" s="2"/>
+    </row>
+    <row r="289" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D289" s="2"/>
+    </row>
+    <row r="290" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D290" s="2"/>
+    </row>
+    <row r="291" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D291" s="2"/>
+    </row>
+    <row r="292" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D292" s="2"/>
+    </row>
+    <row r="293" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D293" s="2"/>
+    </row>
+    <row r="294" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D294" s="2"/>
+    </row>
+    <row r="295" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D295" s="2"/>
+    </row>
+    <row r="296" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D296" s="2"/>
+    </row>
+    <row r="297" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D297" s="2"/>
+    </row>
+    <row r="298" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D298" s="2"/>
+    </row>
+    <row r="299" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D299" s="2"/>
+    </row>
+    <row r="300" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D300" s="2"/>
+    </row>
+    <row r="301" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D301" s="2"/>
+    </row>
+    <row r="302" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D302" s="2"/>
+    </row>
+    <row r="303" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D303" s="2"/>
+    </row>
+    <row r="304" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D304" s="2"/>
+    </row>
+    <row r="305" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D305" s="2"/>
+    </row>
+    <row r="306" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D306" s="2"/>
+    </row>
+    <row r="307" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D307" s="2"/>
+    </row>
+    <row r="308" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D308" s="2"/>
+    </row>
+    <row r="309" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D309" s="2"/>
+    </row>
+    <row r="310" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D310" s="2"/>
+    </row>
+    <row r="311" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D311" s="2"/>
+    </row>
+    <row r="312" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D312" s="2"/>
+    </row>
+    <row r="313" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D313" s="2"/>
+    </row>
+    <row r="314" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D314" s="2"/>
+    </row>
+    <row r="315" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D315" s="2"/>
+    </row>
+    <row r="316" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D316" s="2"/>
+    </row>
+    <row r="317" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D317" s="2"/>
+    </row>
+    <row r="318" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D318" s="2"/>
+    </row>
+    <row r="319" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D319" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed future pricing for simple equity case and simple commidity case
</commit_message>
<xml_diff>
--- a/financial_derivates_futures_options/reliance_future_dataset.xlsx
+++ b/financial_derivates_futures_options/reliance_future_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_derivates/financial_derivates_futures_options/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC6943A-13C6-334A-A479-F307D26C2CCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72264A1-E334-EE44-A728-65B2379C9839}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{0392D1FD-9317-0E42-BE43-26A2C5832841}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{0392D1FD-9317-0E42-BE43-26A2C5832841}"/>
   </bookViews>
   <sheets>
     <sheet name="Hedging &amp; Payoff" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="June - Sep Data" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Futures Data'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Futures Data'!$A$5:$C$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="81">
   <si>
     <t xml:space="preserve">DATE </t>
   </si>
@@ -261,6 +261,21 @@
   <si>
     <t>Spot price on 24th Sep</t>
   </si>
+  <si>
+    <t>RIL Futures Margin</t>
+  </si>
+  <si>
+    <t>Zerodha Margin Calculator</t>
+  </si>
+  <si>
+    <t>Margin Requires</t>
+  </si>
+  <si>
+    <t>Margin Cash Flow</t>
+  </si>
+  <si>
+    <t>MTM Proft / Losses</t>
+  </si>
 </sst>
 </file>
 
@@ -332,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -340,6 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +453,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Futures Data'!$D$1</c:f>
+              <c:f>'Futures Data'!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -472,7 +488,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Futures Data'!$A$2:$A$61</c:f>
+              <c:f>'Futures Data'!$A$6:$A$65</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="60"/>
@@ -661,7 +677,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Futures Data'!$C$2:$C$60</c:f>
+              <c:f>'Futures Data'!$C$6:$C$64</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="59"/>
@@ -884,7 +900,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Futures Data'!$A$2:$A$60</c:f>
+              <c:f>'Futures Data'!$A$6:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="59"/>
@@ -1070,7 +1086,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Futures Data'!$D$2:$D$60</c:f>
+              <c:f>'Futures Data'!$D$6:$D$64</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="59"/>
@@ -2033,16 +2049,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>82550</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2371,7 +2387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BC4E22-B584-1541-8E78-A80684393DC6}">
   <dimension ref="A7:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
@@ -2457,7 +2473,7 @@
         <v>44</v>
       </c>
       <c r="C22" s="3">
-        <f>'Futures Data'!D21</f>
+        <f>'Futures Data'!D25</f>
         <v>1426.95</v>
       </c>
       <c r="D22" t="s">
@@ -2483,7 +2499,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" s="5">
-        <f>'Futures Data'!D60</f>
+        <f>'Futures Data'!D64</f>
         <v>1717.9</v>
       </c>
       <c r="C25" s="5">
@@ -2539,7 +2555,7 @@
         <v>55</v>
       </c>
       <c r="C34" s="3">
-        <f>'Futures Data'!C41</f>
+        <f>'Futures Data'!C45</f>
         <v>1459.15</v>
       </c>
       <c r="D34" t="str">
@@ -2605,11 +2621,11 @@
         <v>68</v>
       </c>
       <c r="D45" s="2">
-        <f>'Futures Data'!C9</f>
+        <f>'Futures Data'!C13</f>
         <v>1230</v>
       </c>
       <c r="E45" s="2">
-        <f>'Futures Data'!D9</f>
+        <f>'Futures Data'!D13</f>
         <v>1219.95</v>
       </c>
     </row>
@@ -2621,7 +2637,7 @@
         <v>70</v>
       </c>
       <c r="D46" s="2">
-        <f>'Futures Data'!C60</f>
+        <f>'Futures Data'!C64</f>
         <v>1717.9</v>
       </c>
       <c r="F46" s="2">
@@ -2637,7 +2653,7 @@
         <v>68</v>
       </c>
       <c r="D47" s="2">
-        <f>'Futures Data'!C61</f>
+        <f>'Futures Data'!C65</f>
         <v>1748.3</v>
       </c>
     </row>
@@ -2649,7 +2665,7 @@
         <v>70</v>
       </c>
       <c r="D48" s="2">
-        <f>'Futures Data'!C125</f>
+        <f>'Futures Data'!C129</f>
         <v>2181.1999999999998</v>
       </c>
       <c r="F48" s="2">
@@ -2680,7 +2696,7 @@
         <v>75</v>
       </c>
       <c r="F53" s="2">
-        <f>'Futures Data'!D125</f>
+        <f>'Futures Data'!D129</f>
         <v>2181.1999999999998</v>
       </c>
     </row>
@@ -2697,1773 +2713,2739 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD808CD-D11A-2A44-A93C-B1CA4C3A65E2}">
-  <dimension ref="A1:D125"/>
+  <dimension ref="A2:G129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D61" sqref="D61:D125"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>43917</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44007</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1082</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1065.5999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>43920</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44007</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1045</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1030.45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>43921</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44007</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1122.55</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1113.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>43922</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44007</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1090.55</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1080.45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>43924</v>
       </c>
       <c r="B6" s="1">
         <v>44007</v>
       </c>
       <c r="C6" s="2">
-        <v>1092.55</v>
+        <v>1082</v>
       </c>
       <c r="D6" s="2">
-        <v>1077.45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1065.5999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>43928</v>
+        <v>43920</v>
       </c>
       <c r="B7" s="1">
         <v>44007</v>
       </c>
       <c r="C7" s="2">
-        <v>1219.95</v>
+        <v>1045</v>
       </c>
       <c r="D7" s="2">
-        <v>1206.0999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1030.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>43929</v>
+        <v>43921</v>
       </c>
       <c r="B8" s="1">
         <v>44007</v>
       </c>
       <c r="C8" s="2">
-        <v>1198.5</v>
+        <v>1122.55</v>
       </c>
       <c r="D8" s="2">
-        <v>1192.1500000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1113.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>43930</v>
+        <v>43922</v>
       </c>
       <c r="B9" s="1">
         <v>44007</v>
       </c>
       <c r="C9" s="2">
-        <v>1230</v>
+        <v>1090.55</v>
       </c>
       <c r="D9" s="2">
-        <v>1219.95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1080.45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>43934</v>
+        <v>43924</v>
       </c>
       <c r="B10" s="1">
         <v>44007</v>
       </c>
       <c r="C10" s="2">
-        <v>1201.5999999999999</v>
+        <v>1092.55</v>
       </c>
       <c r="D10" s="2">
-        <v>1189.1500000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1077.45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>43936</v>
+        <v>43928</v>
       </c>
       <c r="B11" s="1">
         <v>44007</v>
       </c>
       <c r="C11" s="2">
-        <v>1160.5</v>
+        <v>1219.95</v>
       </c>
       <c r="D11" s="2">
-        <v>1149.8499999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1206.0999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>43937</v>
+        <v>43929</v>
       </c>
       <c r="B12" s="1">
         <v>44007</v>
       </c>
       <c r="C12" s="2">
-        <v>1181.5999999999999</v>
+        <v>1198.5</v>
       </c>
       <c r="D12" s="2">
-        <v>1168.05</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1192.1500000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>43938</v>
+        <v>43930</v>
       </c>
       <c r="B13" s="1">
         <v>44007</v>
       </c>
       <c r="C13" s="2">
-        <v>1238.95</v>
+        <v>1230</v>
       </c>
       <c r="D13" s="2">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1219.95</v>
+      </c>
+      <c r="E13">
+        <f>C13*C2</f>
+        <v>307.5</v>
+      </c>
+      <c r="F13">
+        <f>-E13</f>
+        <v>-307.5</v>
+      </c>
+      <c r="G13">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>43941</v>
+        <v>43934</v>
       </c>
       <c r="B14" s="1">
         <v>44007</v>
       </c>
       <c r="C14" s="2">
-        <v>1255.1500000000001</v>
+        <v>1201.5999999999999</v>
       </c>
       <c r="D14" s="2">
-        <v>1243.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1189.1500000000001</v>
+      </c>
+      <c r="E14">
+        <f>C14*C2</f>
+        <v>300.39999999999998</v>
+      </c>
+      <c r="F14">
+        <f>E14-E13</f>
+        <v>-7.1000000000000227</v>
+      </c>
+      <c r="G14" s="2">
+        <f>C13-C14</f>
+        <v>28.400000000000091</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>43942</v>
+        <v>43936</v>
       </c>
       <c r="B15" s="1">
         <v>44007</v>
       </c>
       <c r="C15" s="2">
-        <v>1253.8</v>
+        <v>1160.5</v>
       </c>
       <c r="D15" s="2">
-        <v>1237.3499999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1149.8499999999999</v>
+      </c>
+      <c r="E15">
+        <f>C15*C2</f>
+        <v>290.125</v>
+      </c>
+      <c r="F15">
+        <f>E14-E15</f>
+        <v>10.274999999999977</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>43943</v>
+        <v>43937</v>
       </c>
       <c r="B16" s="1">
         <v>44007</v>
       </c>
       <c r="C16" s="2">
-        <v>1369.4</v>
+        <v>1181.5999999999999</v>
       </c>
       <c r="D16" s="2">
-        <v>1363.6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1168.05</v>
+      </c>
+      <c r="E16">
+        <f>C16*$C$2</f>
+        <v>295.39999999999998</v>
+      </c>
+      <c r="F16">
+        <f>E15-E16</f>
+        <v>-5.2749999999999773</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>43944</v>
+        <v>43938</v>
       </c>
       <c r="B17" s="1">
         <v>44007</v>
       </c>
       <c r="C17" s="2">
-        <v>1380.5</v>
+        <v>1238.95</v>
       </c>
       <c r="D17" s="2">
-        <v>1370.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1224</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:E80" si="0">C17*$C$2</f>
+        <v>309.73750000000001</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:F80" si="1">E16-E17</f>
+        <v>-14.337500000000034</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>43945</v>
+        <v>43941</v>
       </c>
       <c r="B18" s="1">
         <v>44007</v>
       </c>
       <c r="C18" s="2">
-        <v>1426</v>
+        <v>1255.1500000000001</v>
       </c>
       <c r="D18" s="2">
-        <v>1417</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1243.8</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>313.78750000000002</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>-4.0500000000000114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>43948</v>
+        <v>43942</v>
       </c>
       <c r="B19" s="1">
         <v>44007</v>
       </c>
       <c r="C19" s="2">
-        <v>1439.7</v>
+        <v>1253.8</v>
       </c>
       <c r="D19" s="2">
-        <v>1429.75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1237.3499999999999</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>313.45</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0.33750000000003411</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>43949</v>
+        <v>43943</v>
       </c>
       <c r="B20" s="1">
         <v>44007</v>
       </c>
       <c r="C20" s="2">
-        <v>1432.1</v>
+        <v>1369.4</v>
       </c>
       <c r="D20" s="2">
-        <v>1428.15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1363.6</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>342.35</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>-28.900000000000034</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>43950</v>
+        <v>43944</v>
       </c>
       <c r="B21" s="1">
         <v>44007</v>
       </c>
       <c r="C21" s="2">
-        <v>1427.8</v>
+        <v>1380.5</v>
       </c>
       <c r="D21" s="2">
-        <v>1426.95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1370.9</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>345.125</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>-2.7749999999999773</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>43951</v>
+        <v>43945</v>
       </c>
       <c r="B22" s="1">
         <v>44007</v>
       </c>
       <c r="C22" s="2">
-        <v>1464.85</v>
+        <v>1426</v>
       </c>
       <c r="D22" s="2">
-        <v>1466</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1417</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>356.5</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>-11.375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>43955</v>
+        <v>43948</v>
       </c>
       <c r="B23" s="1">
         <v>44007</v>
       </c>
       <c r="C23" s="2">
-        <v>1442.65</v>
+        <v>1439.7</v>
       </c>
       <c r="D23" s="2">
-        <v>1435.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1429.75</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>359.92500000000001</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>-3.4250000000000114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>43956</v>
+        <v>43949</v>
       </c>
       <c r="B24" s="1">
         <v>44007</v>
       </c>
       <c r="C24" s="2">
-        <v>1464.4</v>
+        <v>1432.1</v>
       </c>
       <c r="D24" s="2">
-        <v>1460.65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1428.15</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>358.02499999999998</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>1.9000000000000341</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>43957</v>
+        <v>43950</v>
       </c>
       <c r="B25" s="1">
         <v>44007</v>
       </c>
       <c r="C25" s="2">
-        <v>1464.15</v>
+        <v>1427.8</v>
       </c>
       <c r="D25" s="2">
-        <v>1460.75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1426.95</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>356.95</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>1.0749999999999886</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>43958</v>
+        <v>43951</v>
       </c>
       <c r="B26" s="1">
         <v>44007</v>
       </c>
       <c r="C26" s="2">
-        <v>1511.85</v>
+        <v>1464.85</v>
       </c>
       <c r="D26" s="2">
-        <v>1506.95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1466</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>366.21249999999998</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>-9.2624999999999886</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>43959</v>
+        <v>43955</v>
       </c>
       <c r="B27" s="1">
         <v>44007</v>
       </c>
       <c r="C27" s="2">
-        <v>1552.45</v>
+        <v>1442.65</v>
       </c>
       <c r="D27" s="2">
-        <v>1561.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1435.2</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>360.66250000000002</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>5.5499999999999545</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>43962</v>
+        <v>43956</v>
       </c>
       <c r="B28" s="1">
         <v>44007</v>
       </c>
       <c r="C28" s="2">
-        <v>1568.95</v>
+        <v>1464.4</v>
       </c>
       <c r="D28" s="2">
-        <v>1576.8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1460.65</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>366.1</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>-5.4375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>43963</v>
+        <v>43957</v>
       </c>
       <c r="B29" s="1">
         <v>44007</v>
       </c>
       <c r="C29" s="2">
-        <v>1482.2</v>
+        <v>1464.15</v>
       </c>
       <c r="D29" s="2">
-        <v>1479.25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1460.75</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>366.03750000000002</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>43964</v>
+        <v>43958</v>
       </c>
       <c r="B30" s="1">
         <v>44007</v>
       </c>
       <c r="C30" s="2">
-        <v>1497.75</v>
+        <v>1511.85</v>
       </c>
       <c r="D30" s="2">
-        <v>1496.45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1506.95</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>377.96249999999998</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>-11.924999999999955</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>43965</v>
+        <v>43959</v>
       </c>
       <c r="B31" s="1">
         <v>44007</v>
       </c>
       <c r="C31" s="2">
-        <v>1440.5</v>
+        <v>1552.45</v>
       </c>
       <c r="D31" s="2">
-        <v>1435.95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1561.8</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>388.11250000000001</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>-10.150000000000034</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>43966</v>
+        <v>43962</v>
       </c>
       <c r="B32" s="1">
         <v>44007</v>
       </c>
       <c r="C32" s="2">
-        <v>1462.95</v>
+        <v>1568.95</v>
       </c>
       <c r="D32" s="2">
-        <v>1459.4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1576.8</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>392.23750000000001</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>-4.125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>43969</v>
+        <v>43963</v>
       </c>
       <c r="B33" s="1">
         <v>44007</v>
       </c>
       <c r="C33" s="2">
-        <v>1441.8</v>
+        <v>1482.2</v>
       </c>
       <c r="D33" s="2">
-        <v>1440.75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1479.25</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>370.55</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>21.6875</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>43970</v>
+        <v>43964</v>
       </c>
       <c r="B34" s="1">
         <v>44007</v>
       </c>
       <c r="C34" s="2">
-        <v>1410</v>
+        <v>1497.75</v>
       </c>
       <c r="D34" s="2">
-        <v>1408.9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1496.45</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>374.4375</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>-3.8874999999999886</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>43971</v>
+        <v>43965</v>
       </c>
       <c r="B35" s="1">
         <v>44007</v>
       </c>
       <c r="C35" s="2">
-        <v>1433.8</v>
+        <v>1440.5</v>
       </c>
       <c r="D35" s="2">
-        <v>1433.7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1435.95</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>360.125</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>14.3125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>43972</v>
+        <v>43966</v>
       </c>
       <c r="B36" s="1">
         <v>44007</v>
       </c>
       <c r="C36" s="2">
-        <v>1442.45</v>
+        <v>1462.95</v>
       </c>
       <c r="D36" s="2">
-        <v>1441.25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1459.4</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>365.73750000000001</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>-5.6125000000000114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>43973</v>
+        <v>43969</v>
       </c>
       <c r="B37" s="1">
         <v>44007</v>
       </c>
       <c r="C37" s="2">
-        <v>1433.25</v>
+        <v>1441.8</v>
       </c>
       <c r="D37" s="2">
-        <v>1431.55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1440.75</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>360.45</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>5.2875000000000227</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>43977</v>
+        <v>43970</v>
       </c>
       <c r="B38" s="1">
         <v>44007</v>
       </c>
       <c r="C38" s="2">
-        <v>1423.5</v>
+        <v>1410</v>
       </c>
       <c r="D38" s="2">
-        <v>1424.05</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1408.9</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>352.5</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>7.9499999999999886</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>43978</v>
+        <v>43971</v>
       </c>
       <c r="B39" s="1">
         <v>44007</v>
       </c>
       <c r="C39" s="2">
-        <v>1446.2</v>
+        <v>1433.8</v>
       </c>
       <c r="D39" s="2">
-        <v>1445.55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1433.7</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>358.45</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>-5.9499999999999886</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>43979</v>
+        <v>43972</v>
       </c>
       <c r="B40" s="1">
         <v>44007</v>
       </c>
       <c r="C40" s="2">
-        <v>1468.55</v>
+        <v>1442.45</v>
       </c>
       <c r="D40" s="2">
-        <v>1472.25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1441.25</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>360.61250000000001</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>-2.1625000000000227</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>43980</v>
+        <v>43973</v>
       </c>
       <c r="B41" s="1">
         <v>44007</v>
       </c>
       <c r="C41" s="2">
-        <v>1459.15</v>
+        <v>1433.25</v>
       </c>
       <c r="D41" s="2">
-        <v>1464.4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1431.55</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>358.3125</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>2.3000000000000114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>43983</v>
+        <v>43977</v>
       </c>
       <c r="B42" s="1">
         <v>44007</v>
       </c>
       <c r="C42" s="2">
-        <v>1514</v>
+        <v>1423.5</v>
       </c>
       <c r="D42" s="2">
-        <v>1520.35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1424.05</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>355.875</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>2.4375</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>43984</v>
+        <v>43978</v>
       </c>
       <c r="B43" s="1">
         <v>44007</v>
       </c>
       <c r="C43" s="2">
-        <v>1535.5</v>
+        <v>1446.2</v>
       </c>
       <c r="D43" s="2">
-        <v>1535.7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1445.55</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>361.55</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>-5.6750000000000114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>43985</v>
+        <v>43979</v>
       </c>
       <c r="B44" s="1">
         <v>44007</v>
       </c>
       <c r="C44" s="2">
-        <v>1546</v>
+        <v>1468.55</v>
       </c>
       <c r="D44" s="2">
-        <v>1541.65</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1472.25</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>367.13749999999999</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>-5.5874999999999773</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>43986</v>
+        <v>43980</v>
       </c>
       <c r="B45" s="1">
         <v>44007</v>
       </c>
       <c r="C45" s="2">
-        <v>1580.25</v>
+        <v>1459.15</v>
       </c>
       <c r="D45" s="2">
-        <v>1579.8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1464.4</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>364.78750000000002</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>2.3499999999999659</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>43987</v>
+        <v>43983</v>
       </c>
       <c r="B46" s="1">
         <v>44007</v>
       </c>
       <c r="C46" s="2">
-        <v>1581.55</v>
+        <v>1514</v>
       </c>
       <c r="D46" s="2">
-        <v>1581.7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1520.35</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>378.5</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>-13.712499999999977</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>43990</v>
+        <v>43984</v>
       </c>
       <c r="B47" s="1">
         <v>44007</v>
       </c>
       <c r="C47" s="2">
-        <v>1572.7</v>
+        <v>1535.5</v>
       </c>
       <c r="D47" s="2">
-        <v>1569.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1535.7</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>383.875</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>-5.375</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>43991</v>
+        <v>43985</v>
       </c>
       <c r="B48" s="1">
         <v>44007</v>
       </c>
       <c r="C48" s="2">
-        <v>1539.65</v>
+        <v>1546</v>
       </c>
       <c r="D48" s="2">
-        <v>1537.15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1541.65</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>386.5</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>-2.625</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>43992</v>
+        <v>43986</v>
       </c>
       <c r="B49" s="1">
         <v>44007</v>
       </c>
       <c r="C49" s="2">
-        <v>1571.9</v>
+        <v>1580.25</v>
       </c>
       <c r="D49" s="2">
-        <v>1572.15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1579.8</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>395.0625</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>-8.5625</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>43993</v>
+        <v>43987</v>
       </c>
       <c r="B50" s="1">
         <v>44007</v>
       </c>
       <c r="C50" s="2">
-        <v>1540.7</v>
+        <v>1581.55</v>
       </c>
       <c r="D50" s="2">
-        <v>1537.7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1581.7</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>395.38749999999999</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>-0.32499999999998863</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>43994</v>
+        <v>43990</v>
       </c>
       <c r="B51" s="1">
         <v>44007</v>
       </c>
       <c r="C51" s="2">
-        <v>1588.95</v>
+        <v>1572.7</v>
       </c>
       <c r="D51" s="2">
-        <v>1588.8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1569.5</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>393.17500000000001</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>2.2124999999999773</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>43997</v>
+        <v>43991</v>
       </c>
       <c r="B52" s="1">
         <v>44007</v>
       </c>
       <c r="C52" s="2">
-        <v>1617</v>
+        <v>1539.65</v>
       </c>
       <c r="D52" s="2">
-        <v>1614.55</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1537.15</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>384.91250000000002</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>8.2624999999999886</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>43998</v>
+        <v>43992</v>
       </c>
       <c r="B53" s="1">
         <v>44007</v>
       </c>
       <c r="C53" s="2">
-        <v>1615.5</v>
+        <v>1571.9</v>
       </c>
       <c r="D53" s="2">
-        <v>1617.7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1572.15</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>392.97500000000002</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>-8.0625</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>43999</v>
+        <v>43993</v>
       </c>
       <c r="B54" s="1">
         <v>44007</v>
       </c>
       <c r="C54" s="2">
-        <v>1611.7</v>
+        <v>1540.7</v>
       </c>
       <c r="D54" s="2">
-        <v>1615.35</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1537.7</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>385.17500000000001</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="1"/>
+        <v>7.8000000000000114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>44000</v>
+        <v>43994</v>
       </c>
       <c r="B55" s="1">
         <v>44007</v>
       </c>
       <c r="C55" s="2">
-        <v>1654.05</v>
+        <v>1588.95</v>
       </c>
       <c r="D55" s="2">
-        <v>1655.9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1588.8</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>397.23750000000001</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>-12.0625</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>44001</v>
+        <v>43997</v>
       </c>
       <c r="B56" s="1">
         <v>44007</v>
       </c>
       <c r="C56" s="2">
-        <v>1760.35</v>
+        <v>1617</v>
       </c>
       <c r="D56" s="2">
-        <v>1759.4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1614.55</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="0"/>
+        <v>404.25</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>-7.0124999999999886</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>44004</v>
+        <v>43998</v>
       </c>
       <c r="B57" s="1">
         <v>44007</v>
       </c>
       <c r="C57" s="2">
-        <v>1749</v>
+        <v>1615.5</v>
       </c>
       <c r="D57" s="2">
-        <v>1746.15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1617.7</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="0"/>
+        <v>403.875</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>44005</v>
+        <v>43999</v>
       </c>
       <c r="B58" s="1">
         <v>44007</v>
       </c>
       <c r="C58" s="2">
-        <v>1726.4</v>
+        <v>1611.7</v>
       </c>
       <c r="D58" s="2">
-        <v>1720.9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1615.35</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>402.92500000000001</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>0.94999999999998863</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>44006</v>
+        <v>44000</v>
       </c>
       <c r="B59" s="1">
         <v>44007</v>
       </c>
       <c r="C59" s="2">
-        <v>1730.85</v>
+        <v>1654.05</v>
       </c>
       <c r="D59" s="2">
-        <v>1727.85</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1655.9</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>413.51249999999999</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>-10.587499999999977</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>44007</v>
+        <v>44001</v>
       </c>
       <c r="B60" s="1">
         <v>44007</v>
       </c>
       <c r="C60" s="2">
+        <v>1760.35</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1759.4</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>440.08749999999998</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>-26.574999999999989</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>44004</v>
+      </c>
+      <c r="B61" s="1">
+        <v>44007</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1749</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1746.15</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="0"/>
+        <v>437.25</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="1"/>
+        <v>2.8374999999999773</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>44005</v>
+      </c>
+      <c r="B62" s="1">
+        <v>44007</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1726.4</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1720.9</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="0"/>
+        <v>431.6</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>5.6499999999999773</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>44006</v>
+      </c>
+      <c r="B63" s="1">
+        <v>44007</v>
+      </c>
+      <c r="C63" s="2">
+        <v>1730.85</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1727.85</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="0"/>
+        <v>432.71249999999998</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="1"/>
+        <v>-1.1124999999999545</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>44007</v>
+      </c>
+      <c r="B64" s="1">
+        <v>44007</v>
+      </c>
+      <c r="C64" s="2">
         <v>1717.9</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D64" s="2">
         <v>1717.9</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
+      <c r="E64">
+        <f t="shared" si="0"/>
+        <v>429.47500000000002</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="1"/>
+        <v>3.2374999999999545</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
         <v>44008</v>
       </c>
-      <c r="B61" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C61" s="2">
+      <c r="B65" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C65" s="2">
         <v>1748.3</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D65" s="2">
         <v>1741.65</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
+      <c r="E65">
+        <f t="shared" si="0"/>
+        <v>437.07499999999999</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>-7.5999999999999659</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
         <v>44011</v>
       </c>
-      <c r="B62" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C62" s="2">
+      <c r="B66" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C66" s="2">
         <v>1722.95</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D66" s="2">
         <v>1723.15</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
+      <c r="E66">
+        <f t="shared" si="0"/>
+        <v>430.73750000000001</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="1"/>
+        <v>6.3374999999999773</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
         <v>44012</v>
       </c>
-      <c r="B63" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C63" s="2">
+      <c r="B67" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C67" s="2">
         <v>1705</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D67" s="2">
         <v>1704.1</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
+      <c r="E67">
+        <f t="shared" si="0"/>
+        <v>426.25</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="1"/>
+        <v>4.4875000000000114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
         <v>44013</v>
       </c>
-      <c r="B64" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C64" s="2">
+      <c r="B68" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C68" s="2">
         <v>1741.6</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D68" s="2">
         <v>1737.6</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
+      <c r="E68">
+        <f t="shared" si="0"/>
+        <v>435.4</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>-9.1499999999999773</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
         <v>44014</v>
       </c>
-      <c r="B65" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C65" s="2">
+      <c r="B69" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C69" s="2">
         <v>1767.85</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D69" s="2">
         <v>1760.35</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
+      <c r="E69">
+        <f t="shared" si="0"/>
+        <v>441.96249999999998</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>-6.5625</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
         <v>44015</v>
       </c>
-      <c r="B66" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C66" s="2">
+      <c r="B70" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C70" s="2">
         <v>1794</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D70" s="2">
         <v>1787.9</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
+      <c r="E70">
+        <f t="shared" si="0"/>
+        <v>448.5</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>-6.5375000000000227</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
         <v>44018</v>
       </c>
-      <c r="B67" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C67" s="2">
+      <c r="B71" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C71" s="2">
         <v>1858.55</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D71" s="2">
         <v>1851.8</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
+      <c r="E71">
+        <f t="shared" si="0"/>
+        <v>464.63749999999999</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>-16.137499999999989</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
         <v>44019</v>
       </c>
-      <c r="B68" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C68" s="2">
+      <c r="B72" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C72" s="2">
         <v>1838.95</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D72" s="2">
         <v>1823.45</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
+      <c r="E72">
+        <f t="shared" si="0"/>
+        <v>459.73750000000001</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>4.8999999999999773</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
         <v>44020</v>
       </c>
-      <c r="B69" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C69" s="2">
+      <c r="B73" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C73" s="2">
         <v>1813.6</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D73" s="2">
         <v>1798</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="1">
+      <c r="E73">
+        <f t="shared" si="0"/>
+        <v>453.4</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>6.3375000000000341</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
         <v>44021</v>
       </c>
-      <c r="B70" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C70" s="2">
+      <c r="B74" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C74" s="2">
         <v>1836.5</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D74" s="2">
         <v>1824.25</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="1">
+      <c r="E74">
+        <f t="shared" si="0"/>
+        <v>459.125</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>-5.7250000000000227</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
         <v>44022</v>
       </c>
-      <c r="B71" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C71" s="2">
+      <c r="B75" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C75" s="2">
         <v>1895.7</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D75" s="2">
         <v>1878.05</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="1">
+      <c r="E75">
+        <f t="shared" si="0"/>
+        <v>473.92500000000001</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>-14.800000000000011</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
         <v>44025</v>
       </c>
-      <c r="B72" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C72" s="2">
+      <c r="B76" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C76" s="2">
         <v>1950.35</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D76" s="2">
         <v>1935</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="1">
+      <c r="E76">
+        <f t="shared" si="0"/>
+        <v>487.58749999999998</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>-13.662499999999966</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
         <v>44026</v>
       </c>
-      <c r="B73" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C73" s="2">
+      <c r="B77" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C77" s="2">
         <v>1932.35</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D77" s="2">
         <v>1917</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="1">
+      <c r="E77">
+        <f t="shared" si="0"/>
+        <v>483.08749999999998</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
         <v>44027</v>
       </c>
-      <c r="B74" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C74" s="2">
+      <c r="B78" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C78" s="2">
         <v>1861.9</v>
       </c>
-      <c r="D74" s="2">
+      <c r="D78" s="2">
         <v>1844</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="1">
+      <c r="E78">
+        <f t="shared" si="0"/>
+        <v>465.47500000000002</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>17.612499999999955</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
         <v>44028</v>
       </c>
-      <c r="B75" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C75" s="2">
+      <c r="B79" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C79" s="2">
         <v>1853.6</v>
       </c>
-      <c r="D75" s="2">
+      <c r="D79" s="2">
         <v>1843.4</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="1">
+      <c r="E79">
+        <f t="shared" si="0"/>
+        <v>463.4</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>2.0750000000000455</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
         <v>44029</v>
       </c>
-      <c r="B76" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C76" s="2">
+      <c r="B80" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C80" s="2">
         <v>1928.15</v>
       </c>
-      <c r="D76" s="2">
+      <c r="D80" s="2">
         <v>1911.7</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="1">
+      <c r="E80">
+        <f t="shared" si="0"/>
+        <v>482.03750000000002</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>-18.637500000000045</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
         <v>44032</v>
       </c>
-      <c r="B77" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C77" s="2">
+      <c r="B81" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C81" s="2">
         <v>1933.3</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D81" s="2">
         <v>1919.9</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="1">
+      <c r="E81">
+        <f t="shared" ref="E81:E129" si="2">C81*$C$2</f>
+        <v>483.32499999999999</v>
+      </c>
+      <c r="F81">
+        <f t="shared" ref="F81:F129" si="3">E80-E81</f>
+        <v>-1.2874999999999659</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
         <v>44033</v>
       </c>
-      <c r="B78" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C78" s="2">
+      <c r="B82" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C82" s="2">
         <v>1984.05</v>
       </c>
-      <c r="D78" s="2">
+      <c r="D82" s="2">
         <v>1971.55</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="1">
+      <c r="E82">
+        <f t="shared" si="2"/>
+        <v>496.01249999999999</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="3"/>
+        <v>-12.6875</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
         <v>44034</v>
       </c>
-      <c r="B79" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C79" s="2">
+      <c r="B83" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C83" s="2">
         <v>2013.35</v>
       </c>
-      <c r="D79" s="2">
+      <c r="D83" s="2">
         <v>2004</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="1">
+      <c r="E83">
+        <f t="shared" si="2"/>
+        <v>503.33749999999998</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="3"/>
+        <v>-7.3249999999999886</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
         <v>44035</v>
       </c>
-      <c r="B80" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C80" s="2">
+      <c r="B84" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C84" s="2">
         <v>2070.15</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D84" s="2">
         <v>2057.8000000000002</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="1">
+      <c r="E84">
+        <f t="shared" si="2"/>
+        <v>517.53750000000002</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="3"/>
+        <v>-14.200000000000045</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
         <v>44036</v>
       </c>
-      <c r="B81" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C81" s="2">
+      <c r="B85" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C85" s="2">
         <v>2159</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D85" s="2">
         <v>2146.15</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="1">
+      <c r="E85">
+        <f t="shared" si="2"/>
+        <v>539.75</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="3"/>
+        <v>-22.212499999999977</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
         <v>44039</v>
       </c>
-      <c r="B82" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C82" s="2">
+      <c r="B86" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C86" s="2">
         <v>2166.4499999999998</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D86" s="2">
         <v>2156.1999999999998</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="1">
+      <c r="E86">
+        <f t="shared" si="2"/>
+        <v>541.61249999999995</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="3"/>
+        <v>-1.8624999999999545</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
         <v>44040</v>
       </c>
-      <c r="B83" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C83" s="2">
+      <c r="B87" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C87" s="2">
         <v>2187</v>
       </c>
-      <c r="D83" s="2">
+      <c r="D87" s="2">
         <v>2177.6999999999998</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="1">
+      <c r="E87">
+        <f t="shared" si="2"/>
+        <v>546.75</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="3"/>
+        <v>-5.1375000000000455</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
         <v>44041</v>
       </c>
-      <c r="B84" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C84" s="2">
+      <c r="B88" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C88" s="2">
         <v>2114.15</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D88" s="2">
         <v>2096.65</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="1">
+      <c r="E88">
+        <f t="shared" si="2"/>
+        <v>528.53750000000002</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="3"/>
+        <v>18.212499999999977</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
         <v>44042</v>
       </c>
-      <c r="B85" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C85" s="2">
+      <c r="B89" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C89" s="2">
         <v>2120.5</v>
       </c>
-      <c r="D85" s="2">
+      <c r="D89" s="2">
         <v>2108.85</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="1">
+      <c r="E89">
+        <f t="shared" si="2"/>
+        <v>530.125</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="3"/>
+        <v>-1.5874999999999773</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
         <v>44043</v>
       </c>
-      <c r="B86" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C86" s="2">
+      <c r="B90" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C90" s="2">
         <v>2084.5500000000002</v>
       </c>
-      <c r="D86" s="2">
+      <c r="D90" s="2">
         <v>2067.1</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="1">
+      <c r="E90">
+        <f t="shared" si="2"/>
+        <v>521.13750000000005</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="3"/>
+        <v>8.9874999999999545</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
         <v>44046</v>
       </c>
-      <c r="B87" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C87" s="2">
+      <c r="B91" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C91" s="2">
         <v>2025.8</v>
       </c>
-      <c r="D87" s="2">
+      <c r="D91" s="2">
         <v>2009</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="1">
+      <c r="E91">
+        <f t="shared" si="2"/>
+        <v>506.45</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="3"/>
+        <v>14.687500000000057</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
         <v>44047</v>
       </c>
-      <c r="B88" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C88" s="2">
+      <c r="B92" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C92" s="2">
         <v>2167.8000000000002</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D92" s="2">
         <v>2150.6</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="1">
+      <c r="E92">
+        <f t="shared" si="2"/>
+        <v>541.95000000000005</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="3"/>
+        <v>-35.500000000000057</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
         <v>44048</v>
       </c>
-      <c r="B89" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C89" s="2">
+      <c r="B93" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C93" s="2">
         <v>2141.15</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D93" s="2">
         <v>2126.4499999999998</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="1">
+      <c r="E93">
+        <f t="shared" si="2"/>
+        <v>535.28750000000002</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="3"/>
+        <v>6.6625000000000227</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
         <v>44049</v>
       </c>
-      <c r="B90" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C90" s="2">
+      <c r="B94" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C94" s="2">
         <v>2149.9</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D94" s="2">
         <v>2134.1</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="1">
+      <c r="E94">
+        <f t="shared" si="2"/>
+        <v>537.47500000000002</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="3"/>
+        <v>-2.1875</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
         <v>44050</v>
       </c>
-      <c r="B91" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C91" s="2">
+      <c r="B95" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C95" s="2">
         <v>2163.6</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D95" s="2">
         <v>2146.4499999999998</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="1">
+      <c r="E95">
+        <f t="shared" si="2"/>
+        <v>540.9</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="3"/>
+        <v>-3.4249999999999545</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
         <v>44053</v>
       </c>
-      <c r="B92" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C92" s="2">
+      <c r="B96" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C96" s="2">
         <v>2138.35</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D96" s="2">
         <v>2119.85</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="1">
+      <c r="E96">
+        <f t="shared" si="2"/>
+        <v>534.58749999999998</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="3"/>
+        <v>6.3125</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
         <v>44054</v>
       </c>
-      <c r="B93" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C93" s="2">
+      <c r="B97" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C97" s="2">
         <v>2150.65</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D97" s="2">
         <v>2133.8000000000002</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="1">
+      <c r="E97">
+        <f t="shared" si="2"/>
+        <v>537.66250000000002</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="3"/>
+        <v>-3.0750000000000455</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
         <v>44055</v>
       </c>
-      <c r="B94" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C94" s="2">
+      <c r="B98" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C98" s="2">
         <v>2144.1999999999998</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D98" s="2">
         <v>2127.6</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="1">
+      <c r="E98">
+        <f t="shared" si="2"/>
+        <v>536.04999999999995</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="3"/>
+        <v>1.6125000000000682</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
         <v>44056</v>
       </c>
-      <c r="B95" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C95" s="2">
+      <c r="B99" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C99" s="2">
         <v>2137.75</v>
       </c>
-      <c r="D95" s="2">
+      <c r="D99" s="2">
         <v>2122.0500000000002</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" s="1">
+      <c r="E99">
+        <f t="shared" si="2"/>
+        <v>534.4375</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="3"/>
+        <v>1.6124999999999545</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
         <v>44057</v>
       </c>
-      <c r="B96" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C96" s="2">
+      <c r="B100" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C100" s="2">
         <v>2128</v>
       </c>
-      <c r="D96" s="2">
+      <c r="D100" s="2">
         <v>2113.8000000000002</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="1">
+      <c r="E100">
+        <f t="shared" si="2"/>
+        <v>532</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="3"/>
+        <v>2.4375</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
         <v>44060</v>
       </c>
-      <c r="B97" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C97" s="2">
+      <c r="B101" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C101" s="2">
         <v>2104.25</v>
       </c>
-      <c r="D97" s="2">
+      <c r="D101" s="2">
         <v>2091.35</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="1">
+      <c r="E101">
+        <f t="shared" si="2"/>
+        <v>526.0625</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="3"/>
+        <v>5.9375</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
         <v>44061</v>
       </c>
-      <c r="B98" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C98" s="2">
+      <c r="B102" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C102" s="2">
         <v>2131.5500000000002</v>
       </c>
-      <c r="D98" s="2">
+      <c r="D102" s="2">
         <v>2118.5500000000002</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="1">
+      <c r="E102">
+        <f t="shared" si="2"/>
+        <v>532.88750000000005</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="3"/>
+        <v>-6.8250000000000455</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
         <v>44062</v>
       </c>
-      <c r="B99" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C99" s="2">
+      <c r="B103" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C103" s="2">
         <v>2145.25</v>
       </c>
-      <c r="D99" s="2">
+      <c r="D103" s="2">
         <v>2131.5500000000002</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="1">
+      <c r="E103">
+        <f t="shared" si="2"/>
+        <v>536.3125</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="3"/>
+        <v>-3.4249999999999545</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
         <v>44063</v>
       </c>
-      <c r="B100" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C100" s="2">
+      <c r="B104" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C104" s="2">
         <v>2108.15</v>
       </c>
-      <c r="D100" s="2">
+      <c r="D104" s="2">
         <v>2097.0500000000002</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="1">
+      <c r="E104">
+        <f t="shared" si="2"/>
+        <v>527.03750000000002</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="3"/>
+        <v>9.2749999999999773</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
         <v>44064</v>
       </c>
-      <c r="B101" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C101" s="2">
+      <c r="B105" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C105" s="2">
         <v>2093.8000000000002</v>
       </c>
-      <c r="D101" s="2">
+      <c r="D105" s="2">
         <v>2081.85</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="1">
+      <c r="E105">
+        <f t="shared" si="2"/>
+        <v>523.45000000000005</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="3"/>
+        <v>3.5874999999999773</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
         <v>44067</v>
       </c>
-      <c r="B102" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C102" s="2">
+      <c r="B106" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C106" s="2">
         <v>2108.3000000000002</v>
       </c>
-      <c r="D102" s="2">
+      <c r="D106" s="2">
         <v>2095.75</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" s="1">
+      <c r="E106">
+        <f t="shared" si="2"/>
+        <v>527.07500000000005</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="3"/>
+        <v>-3.625</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
         <v>44068</v>
       </c>
-      <c r="B103" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C103" s="2">
+      <c r="B107" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C107" s="2">
         <v>2094</v>
       </c>
-      <c r="D103" s="2">
+      <c r="D107" s="2">
         <v>2082.1</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" s="1">
+      <c r="E107">
+        <f t="shared" si="2"/>
+        <v>523.5</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="3"/>
+        <v>3.5750000000000455</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
         <v>44069</v>
       </c>
-      <c r="B104" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C104" s="2">
+      <c r="B108" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C108" s="2">
         <v>2145.0500000000002</v>
       </c>
-      <c r="D104" s="2">
+      <c r="D108" s="2">
         <v>2137.3000000000002</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" s="1">
+      <c r="E108">
+        <f t="shared" si="2"/>
+        <v>536.26250000000005</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="3"/>
+        <v>-12.762500000000045</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
         <v>44070</v>
       </c>
-      <c r="B105" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C105" s="2">
+      <c r="B109" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C109" s="2">
         <v>2117.1</v>
       </c>
-      <c r="D105" s="2">
+      <c r="D109" s="2">
         <v>2110.6</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" s="1">
+      <c r="E109">
+        <f t="shared" si="2"/>
+        <v>529.27499999999998</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="3"/>
+        <v>6.9875000000000682</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
         <v>44071</v>
       </c>
-      <c r="B106" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C106" s="2">
+      <c r="B110" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C110" s="2">
         <v>2127.1</v>
       </c>
-      <c r="D106" s="2">
+      <c r="D110" s="2">
         <v>2116.15</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" s="1">
+      <c r="E110">
+        <f t="shared" si="2"/>
+        <v>531.77499999999998</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="3"/>
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
         <v>44074</v>
       </c>
-      <c r="B107" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C107" s="2">
+      <c r="B111" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C111" s="2">
         <v>2088.75</v>
       </c>
-      <c r="D107" s="2">
+      <c r="D111" s="2">
         <v>2080.6999999999998</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" s="1">
+      <c r="E111">
+        <f t="shared" si="2"/>
+        <v>522.1875</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="3"/>
+        <v>9.5874999999999773</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
         <v>44075</v>
       </c>
-      <c r="B108" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C108" s="2">
+      <c r="B112" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C112" s="2">
         <v>2100.15</v>
       </c>
-      <c r="D108" s="2">
+      <c r="D112" s="2">
         <v>2087.25</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" s="1">
+      <c r="E112">
+        <f t="shared" si="2"/>
+        <v>525.03750000000002</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="3"/>
+        <v>-2.8500000000000227</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
         <v>44076</v>
       </c>
-      <c r="B109" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C109" s="2">
+      <c r="B113" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C113" s="2">
         <v>2139.5500000000002</v>
       </c>
-      <c r="D109" s="2">
+      <c r="D113" s="2">
         <v>2128.1999999999998</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" s="1">
+      <c r="E113">
+        <f t="shared" si="2"/>
+        <v>534.88750000000005</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="3"/>
+        <v>-9.8500000000000227</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
         <v>44077</v>
       </c>
-      <c r="B110" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C110" s="2">
+      <c r="B114" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C114" s="2">
         <v>2120</v>
       </c>
-      <c r="D110" s="2">
+      <c r="D114" s="2">
         <v>2112.1</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" s="1">
+      <c r="E114">
+        <f t="shared" si="2"/>
+        <v>530</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="3"/>
+        <v>4.8875000000000455</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
         <v>44078</v>
       </c>
-      <c r="B111" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C111" s="2">
+      <c r="B115" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C115" s="2">
         <v>2083.8000000000002</v>
       </c>
-      <c r="D111" s="2">
+      <c r="D115" s="2">
         <v>2077.25</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" s="1">
+      <c r="E115">
+        <f t="shared" si="2"/>
+        <v>520.95000000000005</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="3"/>
+        <v>9.0499999999999545</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
         <v>44081</v>
       </c>
-      <c r="B112" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C112" s="2">
+      <c r="B116" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C116" s="2">
         <v>2097.1</v>
       </c>
-      <c r="D112" s="2">
+      <c r="D116" s="2">
         <v>2082.65</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" s="1">
+      <c r="E116">
+        <f t="shared" si="2"/>
+        <v>524.27499999999998</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="3"/>
+        <v>-3.3249999999999318</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
         <v>44082</v>
       </c>
-      <c r="B113" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C113" s="2">
+      <c r="B117" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C117" s="2">
         <v>2115</v>
       </c>
-      <c r="D113" s="2">
+      <c r="D117" s="2">
         <v>2107.1</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" s="1">
+      <c r="E117">
+        <f t="shared" si="2"/>
+        <v>528.75</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="3"/>
+        <v>-4.4750000000000227</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
         <v>44083</v>
       </c>
-      <c r="B114" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C114" s="2">
+      <c r="B118" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C118" s="2">
         <v>2169.0500000000002</v>
       </c>
-      <c r="D114" s="2">
+      <c r="D118" s="2">
         <v>2161.35</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" s="1">
+      <c r="E118">
+        <f t="shared" si="2"/>
+        <v>542.26250000000005</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="3"/>
+        <v>-13.512500000000045</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
         <v>44084</v>
       </c>
-      <c r="B115" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C115" s="2">
+      <c r="B119" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C119" s="2">
         <v>2316.3000000000002</v>
       </c>
-      <c r="D115" s="2">
+      <c r="D119" s="2">
         <v>2314</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" s="1">
+      <c r="E119">
+        <f t="shared" si="2"/>
+        <v>579.07500000000005</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="3"/>
+        <v>-36.8125</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
         <v>44085</v>
       </c>
-      <c r="B116" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C116" s="2">
+      <c r="B120" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C120" s="2">
         <v>2320.1</v>
       </c>
-      <c r="D116" s="2">
+      <c r="D120" s="2">
         <v>2319.75</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" s="1">
+      <c r="E120">
+        <f t="shared" si="2"/>
+        <v>580.02499999999998</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="3"/>
+        <v>-0.94999999999993179</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
         <v>44088</v>
       </c>
-      <c r="B117" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C117" s="2">
+      <c r="B121" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C121" s="2">
         <v>2303.75</v>
       </c>
-      <c r="D117" s="2">
+      <c r="D121" s="2">
         <v>2302.5500000000002</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" s="1">
+      <c r="E121">
+        <f t="shared" si="2"/>
+        <v>575.9375</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="3"/>
+        <v>4.0874999999999773</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
         <v>44089</v>
       </c>
-      <c r="B118" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C118" s="2">
+      <c r="B122" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C122" s="2">
         <v>2320.5</v>
       </c>
-      <c r="D118" s="2">
+      <c r="D122" s="2">
         <v>2318.85</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A119" s="1">
+      <c r="E122">
+        <f t="shared" si="2"/>
+        <v>580.125</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="3"/>
+        <v>-4.1875</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
         <v>44090</v>
       </c>
-      <c r="B119" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C119" s="2">
+      <c r="B123" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C123" s="2">
         <v>2330.85</v>
       </c>
-      <c r="D119" s="2">
+      <c r="D123" s="2">
         <v>2324.5500000000002</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" s="1">
+      <c r="E123">
+        <f t="shared" si="2"/>
+        <v>582.71249999999998</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="3"/>
+        <v>-2.5874999999999773</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
         <v>44091</v>
       </c>
-      <c r="B120" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C120" s="2">
+      <c r="B124" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C124" s="2">
         <v>2305.6999999999998</v>
       </c>
-      <c r="D120" s="2">
+      <c r="D124" s="2">
         <v>2298.75</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121" s="1">
+      <c r="E124">
+        <f t="shared" si="2"/>
+        <v>576.42499999999995</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="3"/>
+        <v>6.2875000000000227</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
         <v>44092</v>
       </c>
-      <c r="B121" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C121" s="2">
+      <c r="B125" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C125" s="2">
         <v>2307.8000000000002</v>
       </c>
-      <c r="D121" s="2">
+      <c r="D125" s="2">
         <v>2305.6999999999998</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A122" s="1">
+      <c r="E125">
+        <f t="shared" si="2"/>
+        <v>576.95000000000005</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="3"/>
+        <v>-0.52500000000009095</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
         <v>44095</v>
       </c>
-      <c r="B122" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C122" s="2">
+      <c r="B126" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C126" s="2">
         <v>2259.85</v>
       </c>
-      <c r="D122" s="2">
+      <c r="D126" s="2">
         <v>2255.85</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A123" s="1">
+      <c r="E126">
+        <f t="shared" si="2"/>
+        <v>564.96249999999998</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="3"/>
+        <v>11.987500000000068</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
         <v>44096</v>
       </c>
-      <c r="B123" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C123" s="2">
+      <c r="B127" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C127" s="2">
         <v>2218.3000000000002</v>
       </c>
-      <c r="D123" s="2">
+      <c r="D127" s="2">
         <v>2211.15</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A124" s="1">
+      <c r="E127">
+        <f t="shared" si="2"/>
+        <v>554.57500000000005</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="3"/>
+        <v>10.387499999999932</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
         <v>44097</v>
       </c>
-      <c r="B124" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C124" s="2">
+      <c r="B128" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C128" s="2">
         <v>2237.5500000000002</v>
       </c>
-      <c r="D124" s="2">
+      <c r="D128" s="2">
         <v>2230.8000000000002</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A125" s="1">
-        <v>44098</v>
-      </c>
-      <c r="B125" s="1">
-        <v>44098</v>
-      </c>
-      <c r="C125" s="2">
+      <c r="E128">
+        <f t="shared" si="2"/>
+        <v>559.38750000000005</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="3"/>
+        <v>-4.8125</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>44098</v>
+      </c>
+      <c r="B129" s="1">
+        <v>44098</v>
+      </c>
+      <c r="C129" s="2">
         <v>2181.1999999999998</v>
       </c>
-      <c r="D125" s="2">
+      <c r="D129" s="2">
         <v>2181.1999999999998</v>
       </c>
+      <c r="E129">
+        <f t="shared" si="2"/>
+        <v>545.29999999999995</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="3"/>
+        <v>14.087500000000091</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{8E5E01B1-3000-3748-817D-EE67305C683D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
-      <sortCondition ref="A1:A60"/>
+  <autoFilter ref="A5:C5" xr:uid="{8E5E01B1-3000-3748-817D-EE67305C683D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:C64">
+      <sortCondition ref="A5:A64"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>